<commit_message>
almost fully working betting
</commit_message>
<xml_diff>
--- a/WeekGamesTemplate.xlsx
+++ b/WeekGamesTemplate.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doarni\PycharmProjects\EECE4081\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="48" windowWidth="22992" windowHeight="10032"/>
   </bookViews>
   <sheets>
     <sheet name="Games" sheetId="1" r:id="rId1"/>
@@ -182,7 +187,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -572,6 +577,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -611,19 +629,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,6 +638,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -681,7 +689,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -716,7 +724,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -927,45 +935,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C20" sqref="C20:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="20"/>
-    </row>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="21"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="23"/>
-    </row>
-    <row r="3" spans="2:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="25"/>
+    </row>
+    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="28"/>
+    </row>
+    <row r="3" spans="2:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="1"/>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="2:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -982,7 +990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
@@ -999,7 +1007,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B6" s="8" t="s">
         <v>19</v>
       </c>
@@ -1016,7 +1024,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
@@ -1033,7 +1041,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B8" s="12" t="s">
         <v>23</v>
       </c>
@@ -1050,7 +1058,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B9" s="8" t="s">
         <v>25</v>
       </c>
@@ -1067,7 +1075,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B10" s="12" t="s">
         <v>28</v>
       </c>
@@ -1084,7 +1092,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B11" s="12" t="s">
         <v>21</v>
       </c>
@@ -1101,7 +1109,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B12" s="8" t="s">
         <v>31</v>
       </c>
@@ -1118,7 +1126,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B13" s="12" t="s">
         <v>33</v>
       </c>
@@ -1135,7 +1143,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B14" s="12" t="s">
         <v>36</v>
       </c>
@@ -1152,7 +1160,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B15" s="8" t="s">
         <v>34</v>
       </c>
@@ -1169,7 +1177,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B16" s="8" t="s">
         <v>11</v>
       </c>
@@ -1186,7 +1194,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B17" s="12" t="s">
         <v>14</v>
       </c>
@@ -1203,7 +1211,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="13" t="s">
         <v>13</v>
       </c>
@@ -1220,29 +1228,29 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="28" t="s">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="30"/>
       <c r="F20" s="17"/>
     </row>
-    <row r="21" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="29"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="27"/>
+    <row r="21" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="34"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="32"/>
       <c r="F21" s="17"/>
     </row>
   </sheetData>
@@ -1261,80 +1269,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="20"/>
-    </row>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="21"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="23"/>
-    </row>
-    <row r="3" spans="2:8" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
+    </row>
+    <row r="3" spans="2:8" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:8" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="31" t="s">
+    <row r="4" spans="2:8" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="35"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="6">
         <v>12.5</v>
       </c>
@@ -1349,7 +1357,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B6" s="8" t="s">
         <v>19</v>
       </c>
@@ -1368,7 +1376,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
@@ -1387,7 +1395,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B8" s="12" t="s">
         <v>23</v>
       </c>
@@ -1406,7 +1414,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B9" s="8" t="s">
         <v>25</v>
       </c>
@@ -1425,7 +1433,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B10" s="12" t="s">
         <v>28</v>
       </c>
@@ -1444,7 +1452,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B11" s="12" t="s">
         <v>21</v>
       </c>
@@ -1463,7 +1471,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B12" s="8" t="s">
         <v>31</v>
       </c>
@@ -1482,7 +1490,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B13" s="12" t="s">
         <v>33</v>
       </c>
@@ -1501,7 +1509,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B14" s="12" t="s">
         <v>36</v>
       </c>
@@ -1520,7 +1528,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B15" s="8" t="s">
         <v>34</v>
       </c>
@@ -1539,7 +1547,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B16" s="8" t="s">
         <v>11</v>
       </c>
@@ -1558,7 +1566,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B17" s="12" t="s">
         <v>14</v>
       </c>
@@ -1577,7 +1585,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:8" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="13" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
working bet feature (held together by, tape, glue, and my hopes and dreams)
</commit_message>
<xml_diff>
--- a/WeekGamesTemplate.xlsx
+++ b/WeekGamesTemplate.xlsx
@@ -15,12 +15,12 @@
     <sheet name="Games" sheetId="1" r:id="rId1"/>
     <sheet name="Scores" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="54">
   <si>
     <t>Favorite</t>
   </si>
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t>Game of the Week</t>
-  </si>
-  <si>
-    <t>Arizona vs. Missouri</t>
   </si>
   <si>
     <r>
@@ -182,6 +179,30 @@
   </si>
   <si>
     <t>Underdog Score</t>
+  </si>
+  <si>
+    <t>Mon 11/19 07:00 AM</t>
+  </si>
+  <si>
+    <t>Tue 11/20 07:00 AM</t>
+  </si>
+  <si>
+    <t>Wed 11/21 07:00 AM</t>
+  </si>
+  <si>
+    <t>Thu 11/22 07:00 AM</t>
+  </si>
+  <si>
+    <t>Fri 11/23 07:00 AM</t>
+  </si>
+  <si>
+    <t>Sat 11/24 07:00 AM</t>
+  </si>
+  <si>
+    <t>Sun 11/25 07:00 AM</t>
+  </si>
+  <si>
+    <t>Toledo vs. North Texas</t>
   </si>
 </sst>
 </file>
@@ -237,7 +258,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -270,51 +291,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -552,44 +528,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -599,34 +575,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -933,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F21"/>
+  <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:E21"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -946,312 +916,317 @@
     <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="23" t="s">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="25"/>
-    </row>
-    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="26"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
-    </row>
-    <row r="3" spans="2:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
+    </row>
+    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25"/>
+    </row>
+    <row r="3" spans="2:10" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B3" s="1"/>
-      <c r="C3" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
+      <c r="C3" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="2:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="2:10" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="B4" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="33" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B5" s="5" t="s">
-        <v>16</v>
+    <row r="5" spans="2:10" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="B5" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="C5" s="6">
-        <v>12.5</v>
+        <v>11</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B6" s="8" t="s">
+      <c r="F5" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="B6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="6">
+        <v>15.5</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6">
+        <v>5.5</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="B8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="6">
+        <v>12.5</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="B9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="6">
+        <v>5.5</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="2:10" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="B10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="6">
+        <v>14</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="B11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="B12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="B13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6">
+        <v>10.5</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="B14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6">
+        <v>11.5</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="B15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="B16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="6">
+        <v>6.5</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="B17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="B18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="9">
-        <v>11</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="C18" s="6">
+        <v>9.5</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="9">
-        <v>5.5</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B10" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="9">
-        <v>10.5</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B11" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="9">
-        <v>14</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B12" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="9">
-        <v>3.5</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B13" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="9">
-        <v>6.5</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B14" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="9">
-        <v>5.5</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B15" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="9">
-        <v>15.5</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B16" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="9">
-        <v>8.5</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B17" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="9">
-        <v>11.5</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="14">
-        <v>9.5</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>40</v>
+      <c r="F18" s="6" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="29"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="17"/>
+      <c r="C20" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="26"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="14"/>
     </row>
     <row r="21" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="34"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="17"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1285,322 +1260,322 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="26"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="28"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="2:8" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="2:8" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="2:8" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="19" t="s">
+      <c r="D4" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="6">
+      <c r="C5" s="19"/>
+      <c r="D5" s="3">
         <v>12.5</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6" t="s">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="9">
+      <c r="C6" s="7"/>
+      <c r="D6" s="6">
         <v>11</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="9" t="s">
+      <c r="F6" s="7"/>
+      <c r="G6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="9">
+      <c r="C7" s="7"/>
+      <c r="D7" s="6">
         <v>7.5</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="9" t="s">
+      <c r="F7" s="7"/>
+      <c r="G7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="9">
+      <c r="C8" s="7"/>
+      <c r="D8" s="6">
         <v>5.5</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9" t="s">
+      <c r="F8" s="6"/>
+      <c r="G8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="9">
+      <c r="C9" s="7"/>
+      <c r="D9" s="6">
         <v>2.5</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="9" t="s">
+      <c r="F9" s="7"/>
+      <c r="G9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="9">
+      <c r="C10" s="7"/>
+      <c r="D10" s="6">
         <v>10.5</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9" t="s">
+      <c r="F10" s="6"/>
+      <c r="G10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="9">
+      <c r="C11" s="7"/>
+      <c r="D11" s="6">
         <v>14</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9" t="s">
+      <c r="F11" s="6"/>
+      <c r="G11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="9">
+      <c r="C12" s="7"/>
+      <c r="D12" s="6">
         <v>3.5</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="9" t="s">
+      <c r="F12" s="7"/>
+      <c r="G12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="9">
+      <c r="C13" s="7"/>
+      <c r="D13" s="6">
         <v>6.5</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9" t="s">
+      <c r="F13" s="6"/>
+      <c r="G13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="9">
+      <c r="C14" s="7"/>
+      <c r="D14" s="6">
         <v>5.5</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9" t="s">
+      <c r="F14" s="6"/>
+      <c r="G14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="9">
+      <c r="C15" s="7"/>
+      <c r="D15" s="6">
         <v>15.5</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="9" t="s">
+      <c r="F15" s="7"/>
+      <c r="G15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="9">
+      <c r="C16" s="7"/>
+      <c r="D16" s="6">
         <v>8.5</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="9" t="s">
+      <c r="F16" s="7"/>
+      <c r="G16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="9">
+      <c r="C17" s="7"/>
+      <c r="D17" s="6">
         <v>11.5</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9" t="s">
+      <c r="F17" s="6"/>
+      <c r="G17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="14">
+      <c r="C18" s="12"/>
+      <c r="D18" s="11">
         <v>9.5</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="15"/>
-      <c r="G18" s="14" t="s">
+      <c r="F18" s="12"/>
+      <c r="G18" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H18" s="13" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>